<commit_message>
Fix logic conditions in forms
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_rooms/forms/cold_rooms/cold_rooms.xlsx
+++ b/app/config/tables/cold_rooms/forms/cold_rooms/cold_rooms.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37940" windowHeight="19700" tabRatio="500"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -497,281 +497,281 @@
     <t>Year must be between 1950 and the current year or -1 if unknown</t>
   </si>
   <si>
+    <t>display.hint.text.es</t>
+  </si>
+  <si>
+    <t>Enter -1 if year is unknown</t>
+  </si>
+  <si>
+    <t>Ingrese -1 si el año es desconocido</t>
+  </si>
+  <si>
+    <t>serial_number</t>
+  </si>
+  <si>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>Número de serie</t>
+  </si>
+  <si>
+    <t>Enter the serial number:</t>
+  </si>
+  <si>
+    <t>Ingrese el número de serie</t>
+  </si>
+  <si>
+    <t>Functional Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functional status: </t>
+  </si>
+  <si>
+    <t>functional_status</t>
+  </si>
+  <si>
+    <t>data('voltage_regulator') === 'yes'</t>
+  </si>
+  <si>
+    <t>Voltage Regulator Functional</t>
+  </si>
+  <si>
+    <t>voltage_regulator_functional_status</t>
+  </si>
+  <si>
+    <t>Regulador de voltaje funcional</t>
+  </si>
+  <si>
+    <t>Is voltage regulator functional?</t>
+  </si>
+  <si>
+    <t>¿Funciona el regulador de voltaje?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if </t>
+  </si>
+  <si>
+    <t>not_functioning</t>
+  </si>
+  <si>
+    <t>Not Functioning</t>
+  </si>
+  <si>
+    <t>No Functionando</t>
+  </si>
+  <si>
+    <t>yes_no_unknown</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>unknown_needs_investigation</t>
+  </si>
+  <si>
+    <t>Unknown/Needs Investigation</t>
+  </si>
+  <si>
+    <t>Investigación desconocida / de necesidades</t>
+  </si>
+  <si>
+    <t>lack_of_power</t>
+  </si>
+  <si>
+    <t>Lack of Power</t>
+  </si>
+  <si>
+    <t>Falta de poder</t>
+  </si>
+  <si>
+    <t>awaiting_installation</t>
+  </si>
+  <si>
+    <t>Awaiting Installation</t>
+  </si>
+  <si>
+    <t>En espera de instalación</t>
+  </si>
+  <si>
+    <t>awaiting_decomissioning</t>
+  </si>
+  <si>
+    <t>Awaiting Decomissioning</t>
+  </si>
+  <si>
+    <t>En espera de desarme</t>
+  </si>
+  <si>
+    <t>lack_of_tech_availability</t>
+  </si>
+  <si>
+    <t>Lack of Technician Availability</t>
+  </si>
+  <si>
+    <t>Falta de disponibilidad de técnicos</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>1=1</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>health_facilities</t>
+  </si>
+  <si>
+    <t>cold_rooms</t>
+  </si>
+  <si>
+    <t>Cold Rooms</t>
+  </si>
+  <si>
+    <t>Cuartos Fríos</t>
+  </si>
+  <si>
+    <t>config/tables/cold_rooms/html/cold_rooms_detail.html</t>
+  </si>
+  <si>
+    <t>config/tables/cold_rooms/html/cold_rooms_list.html</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>storage_temperature</t>
+  </si>
+  <si>
+    <t>net_volume</t>
+  </si>
+  <si>
+    <t>dimensions</t>
+  </si>
+  <si>
+    <t>backup_generator</t>
+  </si>
+  <si>
+    <t>Backup Generator</t>
+  </si>
+  <si>
+    <t>data('backup_generator') === yes</t>
+  </si>
+  <si>
+    <t>backup_generator_functional_status</t>
+  </si>
+  <si>
+    <t>cold_room_image</t>
+  </si>
+  <si>
+    <t>Cold Room Image</t>
+  </si>
+  <si>
+    <t>Take a picture of the cold room:</t>
+  </si>
+  <si>
+    <t>Backup Generator Functional</t>
+  </si>
+  <si>
+    <t>Storage Temperature</t>
+  </si>
+  <si>
+    <t>Net Volume</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>Temperatura de almacenamiento</t>
+  </si>
+  <si>
+    <t>Enter the storage temperature:</t>
+  </si>
+  <si>
+    <t>Ingrese la temperatura de almacenamiento:</t>
+  </si>
+  <si>
+    <t>Volumen neto</t>
+  </si>
+  <si>
+    <t>Enter the net volume:</t>
+  </si>
+  <si>
+    <t>Ingrese el volumen neto:</t>
+  </si>
+  <si>
+    <t>Dimensiones</t>
+  </si>
+  <si>
+    <t>Enter the dimensions:</t>
+  </si>
+  <si>
+    <t>Ingrese las dimensiones:</t>
+  </si>
+  <si>
+    <t>Imagen del cuarto frio</t>
+  </si>
+  <si>
+    <t>Tome una foto del cuarto frio</t>
+  </si>
+  <si>
+    <t>Generador de respaldo</t>
+  </si>
+  <si>
+    <t>Backup generator?</t>
+  </si>
+  <si>
+    <t>¿Tiene generador de respaldo?</t>
+  </si>
+  <si>
+    <t>Generador de respaldo funcional</t>
+  </si>
+  <si>
+    <t>Is backup generator functional?</t>
+  </si>
+  <si>
+    <t>¿Funciona el generador de respaldo?</t>
+  </si>
+  <si>
+    <t>cold_room_id</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Fabricante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter the manufacturer: </t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Enter the model:</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Enter the type</t>
+  </si>
+  <si>
     <t>(function() {
   var currDate = new Date();
   var currYear = currDate.getFullYear();
-  return (data('year') &gt;= 1950 &amp;&amp; data('year') &lt;= currYear) || data('year') === -1
+  return (data('year') &gt;= 1950 &amp;&amp; data('year') &lt;= currYear) || parseInt(data('year')) === -1
 })()</t>
-  </si>
-  <si>
-    <t>display.hint.text.es</t>
-  </si>
-  <si>
-    <t>Enter -1 if year is unknown</t>
-  </si>
-  <si>
-    <t>Ingrese -1 si el año es desconocido</t>
-  </si>
-  <si>
-    <t>serial_number</t>
-  </si>
-  <si>
-    <t>Serial Number</t>
-  </si>
-  <si>
-    <t>Número de serie</t>
-  </si>
-  <si>
-    <t>Enter the serial number:</t>
-  </si>
-  <si>
-    <t>Ingrese el número de serie</t>
-  </si>
-  <si>
-    <t>Functional Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional status: </t>
-  </si>
-  <si>
-    <t>functional_status</t>
-  </si>
-  <si>
-    <t>data('voltage_regulator') === 'yes'</t>
-  </si>
-  <si>
-    <t>Voltage Regulator Functional</t>
-  </si>
-  <si>
-    <t>voltage_regulator_functional_status</t>
-  </si>
-  <si>
-    <t>Regulador de voltaje funcional</t>
-  </si>
-  <si>
-    <t>Is voltage regulator functional?</t>
-  </si>
-  <si>
-    <t>¿Funciona el regulador de voltaje?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if </t>
-  </si>
-  <si>
-    <t>not_functioning</t>
-  </si>
-  <si>
-    <t>Not Functioning</t>
-  </si>
-  <si>
-    <t>No Functionando</t>
-  </si>
-  <si>
-    <t>yes_no_unknown</t>
-  </si>
-  <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>unknown_needs_investigation</t>
-  </si>
-  <si>
-    <t>Unknown/Needs Investigation</t>
-  </si>
-  <si>
-    <t>Investigación desconocida / de necesidades</t>
-  </si>
-  <si>
-    <t>lack_of_power</t>
-  </si>
-  <si>
-    <t>Lack of Power</t>
-  </si>
-  <si>
-    <t>Falta de poder</t>
-  </si>
-  <si>
-    <t>awaiting_installation</t>
-  </si>
-  <si>
-    <t>Awaiting Installation</t>
-  </si>
-  <si>
-    <t>En espera de instalación</t>
-  </si>
-  <si>
-    <t>awaiting_decomissioning</t>
-  </si>
-  <si>
-    <t>Awaiting Decomissioning</t>
-  </si>
-  <si>
-    <t>En espera de desarme</t>
-  </si>
-  <si>
-    <t>lack_of_tech_availability</t>
-  </si>
-  <si>
-    <t>Lack of Technician Availability</t>
-  </si>
-  <si>
-    <t>Falta de disponibilidad de técnicos</t>
-  </si>
-  <si>
-    <t>No aplica</t>
-  </si>
-  <si>
-    <t>1=1</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>health_facilities</t>
-  </si>
-  <si>
-    <t>cold_rooms</t>
-  </si>
-  <si>
-    <t>Cold Rooms</t>
-  </si>
-  <si>
-    <t>Cuartos Fríos</t>
-  </si>
-  <si>
-    <t>config/tables/cold_rooms/html/cold_rooms_detail.html</t>
-  </si>
-  <si>
-    <t>config/tables/cold_rooms/html/cold_rooms_list.html</t>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>manufacturer</t>
-  </si>
-  <si>
-    <t>storage_temperature</t>
-  </si>
-  <si>
-    <t>net_volume</t>
-  </si>
-  <si>
-    <t>dimensions</t>
-  </si>
-  <si>
-    <t>backup_generator</t>
-  </si>
-  <si>
-    <t>Backup Generator</t>
-  </si>
-  <si>
-    <t>data('backup_generator') === yes</t>
-  </si>
-  <si>
-    <t>backup_generator_functional_status</t>
-  </si>
-  <si>
-    <t>cold_room_image</t>
-  </si>
-  <si>
-    <t>Cold Room Image</t>
-  </si>
-  <si>
-    <t>Take a picture of the cold room:</t>
-  </si>
-  <si>
-    <t>Backup Generator Functional</t>
-  </si>
-  <si>
-    <t>Storage Temperature</t>
-  </si>
-  <si>
-    <t>Net Volume</t>
-  </si>
-  <si>
-    <t>Dimensions</t>
-  </si>
-  <si>
-    <t>Temperatura de almacenamiento</t>
-  </si>
-  <si>
-    <t>Enter the storage temperature:</t>
-  </si>
-  <si>
-    <t>Ingrese la temperatura de almacenamiento:</t>
-  </si>
-  <si>
-    <t>Volumen neto</t>
-  </si>
-  <si>
-    <t>Enter the net volume:</t>
-  </si>
-  <si>
-    <t>Ingrese el volumen neto:</t>
-  </si>
-  <si>
-    <t>Dimensiones</t>
-  </si>
-  <si>
-    <t>Enter the dimensions:</t>
-  </si>
-  <si>
-    <t>Ingrese las dimensiones:</t>
-  </si>
-  <si>
-    <t>Imagen del cuarto frio</t>
-  </si>
-  <si>
-    <t>Tome una foto del cuarto frio</t>
-  </si>
-  <si>
-    <t>Generador de respaldo</t>
-  </si>
-  <si>
-    <t>Backup generator?</t>
-  </si>
-  <si>
-    <t>¿Tiene generador de respaldo?</t>
-  </si>
-  <si>
-    <t>Generador de respaldo funcional</t>
-  </si>
-  <si>
-    <t>Is backup generator functional?</t>
-  </si>
-  <si>
-    <t>¿Funciona el generador de respaldo?</t>
-  </si>
-  <si>
-    <t>cold_room_id</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Fabricante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter the manufacturer: </t>
-  </si>
-  <si>
-    <t>Modelo</t>
-  </si>
-  <si>
-    <t>Enter the model:</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Enter the type</t>
   </si>
 </sst>
 </file>
@@ -1329,28 +1329,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="2" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="25.1796875" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" customWidth="1"/>
-    <col min="7" max="7" width="29.54296875" customWidth="1"/>
-    <col min="8" max="8" width="30.453125" customWidth="1"/>
-    <col min="9" max="9" width="41.54296875" customWidth="1"/>
-    <col min="10" max="10" width="22.81640625" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" customWidth="1"/>
-    <col min="12" max="12" width="20.26953125" customWidth="1"/>
-    <col min="13" max="13" width="16.1796875" customWidth="1"/>
-    <col min="14" max="1026" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="9" width="41.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="1026" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
@@ -1409,14 +1409,14 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>18</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>23</v>
@@ -1458,28 +1458,28 @@
       <c r="D5" s="3"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H6" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="J6" s="16" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
@@ -1488,40 +1488,40 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H7" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>244</v>
-      </c>
       <c r="J7" s="17" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="I8" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="I8" s="16" t="s">
-        <v>240</v>
-      </c>
       <c r="J8" s="16" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
@@ -1545,28 +1545,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" t="s">
         <v>158</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>159</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>160</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>161</v>
       </c>
-      <c r="J10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D11" s="3" t="s">
         <v>145</v>
       </c>
@@ -1587,10 +1587,10 @@
         <v>33</v>
       </c>
       <c r="K11" t="s">
+        <v>155</v>
+      </c>
+      <c r="L11" t="s">
         <v>156</v>
-      </c>
-      <c r="L11" t="s">
-        <v>157</v>
       </c>
       <c r="Q11" t="s">
         <v>150</v>
@@ -1602,117 +1602,117 @@
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="H14" t="s">
+        <v>226</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="I14" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D17" s="3" t="s">
         <v>145</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H17" t="s">
+        <v>217</v>
+      </c>
+      <c r="I17" t="s">
         <v>218</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>219</v>
       </c>
-      <c r="J17" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>145</v>
       </c>
       <c r="F18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H18" t="s">
+        <v>220</v>
+      </c>
+      <c r="I18" t="s">
         <v>221</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>222</v>
       </c>
-      <c r="J18" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H19" t="s">
+        <v>223</v>
+      </c>
+      <c r="I19" t="s">
         <v>224</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>225</v>
       </c>
-      <c r="J19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>24</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>24</v>
       </c>
@@ -1743,22 +1743,22 @@
         <v>41</v>
       </c>
       <c r="F21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H21" t="s">
         <v>42</v>
       </c>
       <c r="I21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>24</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>24</v>
       </c>
@@ -1804,22 +1804,22 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>49</v>
@@ -1837,15 +1837,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>24</v>
       </c>
@@ -1853,68 +1853,68 @@
         <v>41</v>
       </c>
       <c r="F28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G28" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" t="s">
         <v>168</v>
       </c>
-      <c r="G28" t="s">
-        <v>167</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>169</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>170</v>
       </c>
-      <c r="J28" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
         <v>24</v>
       </c>
       <c r="E32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F32" t="s">
+        <v>206</v>
+      </c>
+      <c r="G32" t="s">
         <v>207</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
+        <v>228</v>
+      </c>
+      <c r="I32" t="s">
+        <v>229</v>
+      </c>
+      <c r="J32" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" t="s">
         <v>208</v>
       </c>
-      <c r="H32" t="s">
-        <v>229</v>
-      </c>
-      <c r="I32" t="s">
-        <v>230</v>
-      </c>
-      <c r="J32" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>172</v>
-      </c>
-      <c r="C33" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>24</v>
       </c>
@@ -1922,27 +1922,27 @@
         <v>41</v>
       </c>
       <c r="F34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G34" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H34" t="s">
+        <v>231</v>
+      </c>
+      <c r="I34" t="s">
         <v>232</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>233</v>
       </c>
-      <c r="J34" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>25</v>
       </c>
@@ -1966,15 +1966,15 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="25.1796875" customWidth="1"/>
-    <col min="3" max="3" width="44.1796875" customWidth="1"/>
-    <col min="4" max="1025" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -2002,21 +2002,21 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -2030,77 +2030,77 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" t="s">
         <v>179</v>
       </c>
-      <c r="D6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="D7" t="s">
         <v>182</v>
       </c>
-      <c r="D7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" t="s">
         <v>185</v>
       </c>
-      <c r="D8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="D9" t="s">
         <v>188</v>
       </c>
-      <c r="D9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="D10" t="s">
         <v>191</v>
       </c>
-      <c r="D10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>44</v>
       </c>
@@ -2111,15 +2111,15 @@
         <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -2161,9 +2161,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
         <v>74</v>
@@ -2175,9 +2175,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
         <v>77</v>
@@ -2189,9 +2189,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
@@ -2203,7 +2203,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>129</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="15"/>
     </row>
   </sheetData>
@@ -2281,21 +2281,21 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" customWidth="1"/>
-    <col min="7" max="9" width="39.54296875" customWidth="1"/>
-    <col min="10" max="10" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="9" width="39.5703125" customWidth="1"/>
+    <col min="10" max="10" width="39.42578125" customWidth="1"/>
     <col min="11" max="11" width="43" customWidth="1"/>
-    <col min="12" max="1025" width="10.81640625" customWidth="1"/>
+    <col min="12" max="1025" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>79</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2338,16 +2338,16 @@
         <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
@@ -2378,14 +2378,14 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.81640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="34.453125" style="10" customWidth="1"/>
-    <col min="4" max="1025" width="10.81640625" style="10" customWidth="1"/>
+    <col min="1" max="2" width="10.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="10" customWidth="1"/>
+    <col min="4" max="1025" width="10.85546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>92</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>96</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>96</v>
       </c>
@@ -2433,10 +2433,10 @@
         <v>99</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>96</v>
       </c>
@@ -2450,10 +2450,10 @@
         <v>99</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>96</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>96</v>
       </c>
@@ -2487,14 +2487,14 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>109</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>112</v>
       </c>
@@ -2547,15 +2547,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" customWidth="1"/>
-    <col min="4" max="1025" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="1025" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>115</v>
       </c>
@@ -2575,23 +2575,23 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>120</v>
       </c>
@@ -2599,18 +2599,18 @@
         <v>20191005</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" t="s">
         <v>198</v>
       </c>
-      <c r="D5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -2659,9 +2659,9 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2669,12 +2669,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2696,17 +2696,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.453125" customWidth="1"/>
-    <col min="2" max="2" width="42.81640625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>148</v>
       </c>
@@ -2714,12 +2714,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="100" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>149</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove unnecessary refrigerator_id and add regionName to geographic_regions
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_rooms/forms/cold_rooms/cold_rooms.xlsx
+++ b/app/config/tables/cold_rooms/forms/cold_rooms/cold_rooms.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,9 @@
     <sheet name="queries" sheetId="3" r:id="rId3"/>
     <sheet name="properties" sheetId="4" r:id="rId4"/>
     <sheet name="settings" sheetId="5" r:id="rId5"/>
-    <sheet name="model" sheetId="6" r:id="rId6"/>
-    <sheet name="calculates" sheetId="7" r:id="rId7"/>
+    <sheet name="calculates" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="244">
   <si>
     <t>comments</t>
   </si>
@@ -735,9 +734,6 @@
   </si>
   <si>
     <t>¿Funciona el generador de respaldo?</t>
-  </si>
-  <si>
-    <t>cold_room_id</t>
   </si>
   <si>
     <t>Model</t>
@@ -1329,7 +1325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -1467,16 +1463,16 @@
         <v>201</v>
       </c>
       <c r="G6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H6" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>241</v>
-      </c>
       <c r="J6" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1488,16 +1484,16 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H7" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>243</v>
-      </c>
       <c r="J7" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1509,16 +1505,16 @@
         <v>202</v>
       </c>
       <c r="G8" t="s">
+        <v>236</v>
+      </c>
+      <c r="H8" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="I8" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="I8" s="16" t="s">
-        <v>239</v>
-      </c>
       <c r="J8" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2655,49 +2651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2719,7 +2674,7 @@
         <v>149</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add units to forms and fix logic for grid availability visibility
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_rooms/forms/cold_rooms/cold_rooms.xlsx
+++ b/app/config/tables/cold_rooms/forms/cold_rooms/cold_rooms.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37940" windowHeight="19700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="250">
   <si>
     <t>comments</t>
   </si>
@@ -768,6 +768,24 @@
   </si>
   <si>
     <t>No Instalado</t>
+  </si>
+  <si>
+    <t>(degrees Celsius)</t>
+  </si>
+  <si>
+    <t>(grados Celsius)</t>
+  </si>
+  <si>
+    <t>(cubic meters)</t>
+  </si>
+  <si>
+    <t>(metros cúbicos)</t>
+  </si>
+  <si>
+    <t>(meters)</t>
+  </si>
+  <si>
+    <t>(metros)</t>
   </si>
 </sst>
 </file>
@@ -1325,28 +1343,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
-    <col min="9" max="9" width="41.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" customWidth="1"/>
-    <col min="14" max="1026" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="2" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="25.1796875" customWidth="1"/>
+    <col min="6" max="6" width="24.54296875" customWidth="1"/>
+    <col min="7" max="7" width="29.54296875" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" customWidth="1"/>
+    <col min="9" max="9" width="41.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.81640625" customWidth="1"/>
+    <col min="11" max="11" width="19.54296875" customWidth="1"/>
+    <col min="12" max="12" width="20.26953125" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" customWidth="1"/>
+    <col min="14" max="1026" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1405,14 +1423,14 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -1420,7 +1438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>18</v>
       </c>
@@ -1446,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>23</v>
@@ -1454,7 +1472,7 @@
       <c r="D5" s="3"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1475,7 +1493,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
@@ -1496,7 +1514,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
@@ -1517,7 +1535,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
@@ -1541,7 +1559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
@@ -1562,7 +1580,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="3" t="s">
         <v>142</v>
       </c>
@@ -1598,21 +1616,21 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="15" t="s">
         <v>173</v>
       </c>
@@ -1633,21 +1651,21 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:19" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
         <v>142</v>
       </c>
@@ -1667,8 +1685,14 @@
       <c r="J17" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
+        <v>244</v>
+      </c>
+      <c r="L17" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>142</v>
       </c>
@@ -1687,8 +1711,14 @@
       <c r="J18" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K18" t="s">
+        <v>246</v>
+      </c>
+      <c r="L18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>26</v>
       </c>
@@ -1707,8 +1737,14 @@
       <c r="J19" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K19" t="s">
+        <v>248</v>
+      </c>
+      <c r="L19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>24</v>
       </c>
@@ -1731,7 +1767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>24</v>
       </c>
@@ -1754,7 +1790,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>24</v>
       </c>
@@ -1777,7 +1813,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>24</v>
       </c>
@@ -1800,17 +1836,17 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>24</v>
       </c>
@@ -1833,7 +1869,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>16</v>
       </c>
@@ -1841,7 +1877,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>24</v>
       </c>
@@ -1864,22 +1900,22 @@
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>24</v>
       </c>
@@ -1902,7 +1938,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>168</v>
       </c>
@@ -1910,7 +1946,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>24</v>
       </c>
@@ -1933,12 +1969,12 @@
         <v>230</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>25</v>
       </c>
@@ -1962,15 +1998,15 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" customWidth="1"/>
-    <col min="4" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" customWidth="1"/>
+    <col min="3" max="3" width="44.1796875" customWidth="1"/>
+    <col min="4" max="1025" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1984,7 +2020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1998,7 +2034,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2012,7 +2048,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -2026,7 +2062,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2040,7 +2076,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2054,7 +2090,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -2068,7 +2104,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -2082,7 +2118,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2096,7 +2132,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>44</v>
       </c>
@@ -2110,12 +2146,12 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2129,7 +2165,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2143,7 +2179,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -2157,7 +2193,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>172</v>
       </c>
@@ -2171,7 +2207,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>172</v>
       </c>
@@ -2185,7 +2221,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>172</v>
       </c>
@@ -2199,7 +2235,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -2213,7 +2249,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -2227,7 +2263,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -2241,7 +2277,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>126</v>
       </c>
@@ -2255,7 +2291,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
     </row>
   </sheetData>
@@ -2277,21 +2313,21 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="9" width="39.5703125" customWidth="1"/>
-    <col min="10" max="10" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
+    <col min="7" max="9" width="39.54296875" customWidth="1"/>
+    <col min="10" max="10" width="39.453125" customWidth="1"/>
     <col min="11" max="11" width="43" customWidth="1"/>
-    <col min="12" max="1025" width="10.85546875" customWidth="1"/>
+    <col min="12" max="1025" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>76</v>
       </c>
@@ -2326,7 +2362,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2374,14 +2410,14 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" style="10" customWidth="1"/>
-    <col min="4" max="1025" width="10.85546875" style="10" customWidth="1"/>
+    <col min="1" max="2" width="10.81640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" style="10" customWidth="1"/>
+    <col min="4" max="1025" width="10.81640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>89</v>
       </c>
@@ -2398,7 +2434,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>93</v>
       </c>
@@ -2415,7 +2451,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>93</v>
       </c>
@@ -2432,7 +2468,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>93</v>
       </c>
@@ -2449,7 +2485,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>93</v>
       </c>
@@ -2466,7 +2502,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>93</v>
       </c>
@@ -2483,14 +2519,14 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>106</v>
       </c>
@@ -2507,7 +2543,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>109</v>
       </c>
@@ -2543,15 +2579,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="1025" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="1025" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>112</v>
       </c>
@@ -2571,7 +2607,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>115</v>
       </c>
@@ -2579,7 +2615,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>116</v>
       </c>
@@ -2587,7 +2623,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>117</v>
       </c>
@@ -2595,7 +2631,7 @@
         <v>20191005</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>118</v>
       </c>
@@ -2606,7 +2642,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -2614,7 +2650,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -2625,7 +2661,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -2655,13 +2691,13 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1"/>
+    <col min="2" max="2" width="42.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>145</v>
       </c>
@@ -2669,7 +2705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="100" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
Add notes to refrigerator and cold room to allow for additional identifying information for non-standard equipment
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_rooms/forms/cold_rooms/cold_rooms.xlsx
+++ b/app/config/tables/cold_rooms/forms/cold_rooms/cold_rooms.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37940" windowHeight="19700" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="8" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="299">
   <si>
     <t>comments</t>
   </si>
@@ -919,6 +919,21 @@
   </si>
   <si>
     <t>data('backup_generator') === 'yes'</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Enter notes</t>
+  </si>
+  <si>
+    <t>Introduce notas</t>
   </si>
 </sst>
 </file>
@@ -1503,16 +1518,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.54296875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="19"/>
-    <col min="3" max="3" width="19.54296875" style="19" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" style="19" customWidth="1"/>
-    <col min="5" max="16384" width="9.54296875" style="19"/>
+    <col min="1" max="1" width="17.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="19"/>
+    <col min="3" max="3" width="19.5703125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="19" customWidth="1"/>
+    <col min="5" max="16384" width="9.5703125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -1526,14 +1541,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>220</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
     </row>
-    <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>221</v>
       </c>
@@ -1551,30 +1566,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W37"/>
+  <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
-    <col min="2" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="25.1796875" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" customWidth="1"/>
-    <col min="7" max="7" width="29.54296875" customWidth="1"/>
-    <col min="8" max="9" width="30.453125" customWidth="1"/>
-    <col min="10" max="10" width="41.54296875" customWidth="1"/>
-    <col min="11" max="12" width="22.81640625" customWidth="1"/>
-    <col min="13" max="13" width="19.54296875" customWidth="1"/>
-    <col min="14" max="15" width="20.26953125" customWidth="1"/>
-    <col min="16" max="16" width="16.1796875" customWidth="1"/>
-    <col min="17" max="1029" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="9" width="30.42578125" customWidth="1"/>
+    <col min="10" max="10" width="41.5703125" customWidth="1"/>
+    <col min="11" max="12" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1"/>
+    <col min="14" max="15" width="20.28515625" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="17" max="1029" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1645,14 +1660,14 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -1660,7 +1675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>18</v>
       </c>
@@ -1686,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>23</v>
@@ -1694,7 +1709,7 @@
       <c r="D5" s="3"/>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1717,7 +1732,7 @@
       </c>
       <c r="L6" s="16"/>
     </row>
-    <row r="7" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1742,7 +1757,7 @@
       </c>
       <c r="L7" s="17"/>
     </row>
-    <row r="8" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
@@ -1765,7 +1780,7 @@
       </c>
       <c r="L8" s="16"/>
     </row>
-    <row r="9" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
@@ -1789,7 +1804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
@@ -1810,7 +1825,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D11" s="3" t="s">
         <v>130</v>
       </c>
@@ -1846,21 +1861,21 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" s="3" t="s">
         <v>130</v>
       </c>
@@ -1887,7 +1902,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>130</v>
       </c>
@@ -1913,7 +1928,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>130</v>
       </c>
@@ -1939,7 +1954,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>26</v>
       </c>
@@ -1965,17 +1980,17 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>24</v>
       </c>
@@ -1998,7 +2013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>24</v>
       </c>
@@ -2021,7 +2036,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" s="13" t="s">
         <v>227</v>
       </c>
@@ -2044,7 +2059,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>24</v>
       </c>
@@ -2067,17 +2082,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>24</v>
       </c>
@@ -2100,7 +2115,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>16</v>
       </c>
@@ -2108,7 +2123,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>26</v>
       </c>
@@ -2128,7 +2143,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>24</v>
       </c>
@@ -2151,22 +2166,22 @@
         <v>276</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
         <v>24</v>
       </c>
@@ -2189,7 +2204,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>150</v>
       </c>
@@ -2197,7 +2212,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
         <v>24</v>
       </c>
@@ -2220,14 +2235,34 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" t="s">
+        <v>294</v>
+      </c>
+      <c r="G38" t="s">
+        <v>295</v>
+      </c>
+      <c r="H38" t="s">
+        <v>296</v>
+      </c>
+      <c r="J38" t="s">
+        <v>297</v>
+      </c>
+      <c r="K38" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2249,17 +2284,17 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="25.1796875" customWidth="1"/>
-    <col min="3" max="3" width="44.1796875" customWidth="1"/>
-    <col min="4" max="4" width="26.1796875" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" customWidth="1"/>
-    <col min="6" max="1025" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -2276,7 +2311,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>223</v>
       </c>
@@ -2291,7 +2326,7 @@
       </c>
       <c r="E2" s="23"/>
     </row>
-    <row r="3" spans="1:5" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>223</v>
       </c>
@@ -2306,7 +2341,7 @@
       </c>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:5" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>223</v>
       </c>
@@ -2321,14 +2356,14 @@
       </c>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:5" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="25"/>
       <c r="D5" s="13"/>
       <c r="E5" s="23"/>
     </row>
-    <row r="6" spans="1:5" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>41</v>
       </c>
@@ -2345,7 +2380,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>41</v>
       </c>
@@ -2362,12 +2397,12 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="E8" s="23"/>
     </row>
-    <row r="9" spans="1:5" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>292</v>
       </c>
@@ -2382,7 +2417,7 @@
       </c>
       <c r="E9" s="22"/>
     </row>
-    <row r="10" spans="1:5" s="20" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="20" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>292</v>
       </c>
@@ -2397,7 +2432,7 @@
       </c>
       <c r="E10" s="21"/>
     </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2411,7 +2446,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2425,7 +2460,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2439,7 +2474,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2453,7 +2488,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -2467,7 +2502,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -2481,7 +2516,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>44</v>
       </c>
@@ -2495,7 +2530,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>35</v>
       </c>
@@ -2510,7 +2545,7 @@
       </c>
       <c r="E20" s="21"/>
     </row>
-    <row r="21" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>35</v>
       </c>
@@ -2525,7 +2560,7 @@
       </c>
       <c r="E21" s="21"/>
     </row>
-    <row r="22" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>35</v>
       </c>
@@ -2540,7 +2575,7 @@
       </c>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>35</v>
       </c>
@@ -2555,7 +2590,7 @@
       </c>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>35</v>
       </c>
@@ -2570,8 +2605,8 @@
       </c>
       <c r="E24" s="21"/>
     </row>
-    <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
         <v>151</v>
       </c>
@@ -2585,7 +2620,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
         <v>151</v>
       </c>
@@ -2599,7 +2634,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>151</v>
       </c>
@@ -2613,7 +2648,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -2627,7 +2662,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -2641,7 +2676,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -2655,7 +2690,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -2669,7 +2704,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="15"/>
     </row>
   </sheetData>
@@ -2691,21 +2726,21 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" customWidth="1"/>
-    <col min="7" max="9" width="39.54296875" customWidth="1"/>
-    <col min="10" max="10" width="39.453125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="9" width="39.5703125" customWidth="1"/>
+    <col min="10" max="10" width="39.42578125" customWidth="1"/>
     <col min="11" max="11" width="43" customWidth="1"/>
-    <col min="12" max="1025" width="10.81640625" customWidth="1"/>
+    <col min="12" max="1025" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>64</v>
       </c>
@@ -2740,7 +2775,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2788,14 +2823,14 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.81640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="34.453125" style="10" customWidth="1"/>
-    <col min="4" max="1025" width="10.81640625" style="10" customWidth="1"/>
+    <col min="1" max="2" width="10.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="10" customWidth="1"/>
+    <col min="4" max="1025" width="10.85546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>77</v>
       </c>
@@ -2812,7 +2847,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>81</v>
       </c>
@@ -2829,7 +2864,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>81</v>
       </c>
@@ -2846,7 +2881,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>81</v>
       </c>
@@ -2863,7 +2898,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>81</v>
       </c>
@@ -2880,7 +2915,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>81</v>
       </c>
@@ -2897,14 +2932,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>94</v>
       </c>
@@ -2921,7 +2956,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>97</v>
       </c>
@@ -2957,16 +2992,16 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="20.26953125" customWidth="1"/>
-    <col min="4" max="5" width="17.26953125" customWidth="1"/>
-    <col min="6" max="1026" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="1026" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>100</v>
       </c>
@@ -2992,7 +3027,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>103</v>
       </c>
@@ -3000,7 +3035,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>104</v>
       </c>
@@ -3008,7 +3043,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>105</v>
       </c>
@@ -3016,7 +3051,7 @@
         <v>20191005</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>106</v>
       </c>
@@ -3027,7 +3062,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -3035,7 +3070,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -3049,7 +3084,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -3063,7 +3098,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>252</v>
       </c>
@@ -3096,13 +3131,13 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.453125" customWidth="1"/>
-    <col min="2" max="2" width="42.81640625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>133</v>
       </c>
@@ -3110,7 +3145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="100" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
Use 0 for unknown installation/procurement year
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_rooms/forms/cold_rooms/cold_rooms.xlsx
+++ b/app/config/tables/cold_rooms/forms/cold_rooms/cold_rooms.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37935" windowHeight="19695" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="8" r:id="rId1"/>
@@ -446,21 +446,9 @@
     <t>display.constraint_message.text.es</t>
   </si>
   <si>
-    <t>El año debe ser entre 1950 y el año actual o -1 si se desconoce</t>
-  </si>
-  <si>
-    <t>Year must be between 1950 and the current year or -1 if unknown</t>
-  </si>
-  <si>
     <t>display.hint.text.es</t>
   </si>
   <si>
-    <t>Enter -1 if year is unknown</t>
-  </si>
-  <si>
-    <t>Ingrese -1 si el año es desconocido</t>
-  </si>
-  <si>
     <t>serial_number</t>
   </si>
   <si>
@@ -669,271 +657,283 @@
   </si>
   <si>
     <t>Enter the type</t>
+  </si>
+  <si>
+    <t>(degrees Celsius)</t>
+  </si>
+  <si>
+    <t>(grados Celsius)</t>
+  </si>
+  <si>
+    <t>(cubic meters)</t>
+  </si>
+  <si>
+    <t>(metros cúbicos)</t>
+  </si>
+  <si>
+    <t>(meters)</t>
+  </si>
+  <si>
+    <t>(metros)</t>
+  </si>
+  <si>
+    <t>display.text</t>
+  </si>
+  <si>
+    <t>do section survey</t>
+  </si>
+  <si>
+    <t>goto _finalize</t>
+  </si>
+  <si>
+    <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
+  </si>
+  <si>
+    <t>cold_room_type</t>
+  </si>
+  <si>
+    <t>gross_volume</t>
+  </si>
+  <si>
+    <t>Gross Volume</t>
+  </si>
+  <si>
+    <t>Is temperature monitoring device functional?</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t>installed_in_use</t>
+  </si>
+  <si>
+    <t>Installed - In Use</t>
+  </si>
+  <si>
+    <t>Instalado - En uso</t>
+  </si>
+  <si>
+    <t>installed_not_in_use</t>
+  </si>
+  <si>
+    <t>Installed - Not In Use</t>
+  </si>
+  <si>
+    <t>Instalado - No en uso</t>
+  </si>
+  <si>
+    <t>not_installed_waiting_for_installation</t>
+  </si>
+  <si>
+    <t>Not Installed - Waiting For Installation</t>
+  </si>
+  <si>
+    <t>No instalado - Esperando instalación</t>
+  </si>
+  <si>
+    <t>not_installed_removed_from_service</t>
+  </si>
+  <si>
+    <t>Not installed - Removed From Service</t>
+  </si>
+  <si>
+    <t>No instalado: eliminado del servicio</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Desaparecido</t>
+  </si>
+  <si>
+    <t>No known issues</t>
+  </si>
+  <si>
+    <t>No hay problemas conocidos</t>
+  </si>
+  <si>
+    <t>Needs attention</t>
+  </si>
+  <si>
+    <t>Necesita atención</t>
+  </si>
+  <si>
+    <t>display.title.text.fr</t>
+  </si>
+  <si>
+    <t>display.prompt.text.fr</t>
+  </si>
+  <si>
+    <t>display.hint.text.fr</t>
+  </si>
+  <si>
+    <t>display.constraint_message.text.fr</t>
+  </si>
+  <si>
+    <t>display.locale.text.fr</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>Anglais</t>
+  </si>
+  <si>
+    <t>Espagnol</t>
+  </si>
+  <si>
+    <t>Francais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">French </t>
+  </si>
+  <si>
+    <t>Francés</t>
+  </si>
+  <si>
+    <t>Enter the gross volume:</t>
+  </si>
+  <si>
+    <t>refrigerator</t>
+  </si>
+  <si>
+    <t>freezer</t>
+  </si>
+  <si>
+    <t>refrigerator_freezer</t>
+  </si>
+  <si>
+    <t>Congelador</t>
+  </si>
+  <si>
+    <t>Refrigerador</t>
+  </si>
+  <si>
+    <t>Refrigerador/Congelador</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Freezer</t>
+  </si>
+  <si>
+    <t>Refrigerator/Freezer</t>
+  </si>
+  <si>
+    <t>temperature_monitoring_device</t>
+  </si>
+  <si>
+    <t>Temperature Monitoring Device</t>
+  </si>
+  <si>
+    <t>Is there a temperature monitoring device?</t>
+  </si>
+  <si>
+    <t>Dispositivo de monitoreo de temperatura</t>
+  </si>
+  <si>
+    <t>data('temperature_monitoring_device') === 'yes'</t>
+  </si>
+  <si>
+    <t>temperature_monitoring_device_functional_status</t>
+  </si>
+  <si>
+    <t>Temperature Monitoring Device Functional</t>
+  </si>
+  <si>
+    <t>Dispositivo de monitoreo de temperatura funcional</t>
+  </si>
+  <si>
+    <t>¿Funciona el dispositivo de monitoreo de temperatura?</t>
+  </si>
+  <si>
+    <t>¿Tiene el dispositivo de monitoreo de temperatura?</t>
+  </si>
+  <si>
+    <t>temperature_monitoring_device_type</t>
+  </si>
+  <si>
+    <t>Temperature Monitoring Device Type</t>
+  </si>
+  <si>
+    <t>Tipo de dispositivo de monitoreo de temperatura</t>
+  </si>
+  <si>
+    <t>What type of the temperature monitoring device is present?</t>
+  </si>
+  <si>
+    <t>¿Qué tipo de dispositivo de monitoreo de temperatura está presente?</t>
+  </si>
+  <si>
+    <t>Volúmen bruto</t>
+  </si>
+  <si>
+    <t>Ingrese el volumen bruto:</t>
+  </si>
+  <si>
+    <t>functioning</t>
+  </si>
+  <si>
+    <t>Functioning</t>
+  </si>
+  <si>
+    <t>Fonctionne</t>
+  </si>
+  <si>
+    <t>not_functioning</t>
+  </si>
+  <si>
+    <t>Not Functioning</t>
+  </si>
+  <si>
+    <t>No Functionando</t>
+  </si>
+  <si>
+    <t>Ne fonctionne pas</t>
+  </si>
+  <si>
+    <t>user_friendly_status</t>
+  </si>
+  <si>
+    <t>data('backup_generator') === 'yes'</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Enter notes</t>
+  </si>
+  <si>
+    <t>Introduce notas</t>
   </si>
   <si>
     <t>(function() {
   var currDate = new Date();
   var currYear = currDate.getFullYear();
-  return (data('year') &gt;= 1950 &amp;&amp; data('year') &lt;= currYear) || parseInt(data('year')) === -1
+  return (data('year') &gt;= 1950 &amp;&amp; data('year') &lt;= currYear) || parseInt(data('year')) === 0
 })()</t>
   </si>
   <si>
-    <t>(degrees Celsius)</t>
-  </si>
-  <si>
-    <t>(grados Celsius)</t>
-  </si>
-  <si>
-    <t>(cubic meters)</t>
-  </si>
-  <si>
-    <t>(metros cúbicos)</t>
-  </si>
-  <si>
-    <t>(meters)</t>
-  </si>
-  <si>
-    <t>(metros)</t>
-  </si>
-  <si>
-    <t>display.text</t>
-  </si>
-  <si>
-    <t>do section survey</t>
-  </si>
-  <si>
-    <t>goto _finalize</t>
-  </si>
-  <si>
-    <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
-  </si>
-  <si>
-    <t>cold_room_type</t>
-  </si>
-  <si>
-    <t>gross_volume</t>
-  </si>
-  <si>
-    <t>Gross Volume</t>
-  </si>
-  <si>
-    <t>Is temperature monitoring device functional?</t>
-  </si>
-  <si>
-    <t>select_multiple</t>
-  </si>
-  <si>
-    <t>installed_in_use</t>
-  </si>
-  <si>
-    <t>Installed - In Use</t>
-  </si>
-  <si>
-    <t>Instalado - En uso</t>
-  </si>
-  <si>
-    <t>installed_not_in_use</t>
-  </si>
-  <si>
-    <t>Installed - Not In Use</t>
-  </si>
-  <si>
-    <t>Instalado - No en uso</t>
-  </si>
-  <si>
-    <t>not_installed_waiting_for_installation</t>
-  </si>
-  <si>
-    <t>Not Installed - Waiting For Installation</t>
-  </si>
-  <si>
-    <t>No instalado - Esperando instalación</t>
-  </si>
-  <si>
-    <t>not_installed_removed_from_service</t>
-  </si>
-  <si>
-    <t>Not installed - Removed From Service</t>
-  </si>
-  <si>
-    <t>No instalado: eliminado del servicio</t>
-  </si>
-  <si>
-    <t>missing</t>
-  </si>
-  <si>
-    <t>Missing</t>
-  </si>
-  <si>
-    <t>Desaparecido</t>
-  </si>
-  <si>
-    <t>No known issues</t>
-  </si>
-  <si>
-    <t>No hay problemas conocidos</t>
-  </si>
-  <si>
-    <t>Needs attention</t>
-  </si>
-  <si>
-    <t>Necesita atención</t>
-  </si>
-  <si>
-    <t>display.title.text.fr</t>
-  </si>
-  <si>
-    <t>display.prompt.text.fr</t>
-  </si>
-  <si>
-    <t>display.hint.text.fr</t>
-  </si>
-  <si>
-    <t>display.constraint_message.text.fr</t>
-  </si>
-  <si>
-    <t>display.locale.text.fr</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>Anglais</t>
-  </si>
-  <si>
-    <t>Espagnol</t>
-  </si>
-  <si>
-    <t>Francais</t>
-  </si>
-  <si>
-    <t xml:space="preserve">French </t>
-  </si>
-  <si>
-    <t>Francés</t>
-  </si>
-  <si>
-    <t>Enter the gross volume:</t>
-  </si>
-  <si>
-    <t>refrigerator</t>
-  </si>
-  <si>
-    <t>freezer</t>
-  </si>
-  <si>
-    <t>refrigerator_freezer</t>
-  </si>
-  <si>
-    <t>Congelador</t>
-  </si>
-  <si>
-    <t>Refrigerador</t>
-  </si>
-  <si>
-    <t>Refrigerador/Congelador</t>
-  </si>
-  <si>
-    <t>Refrigerator</t>
-  </si>
-  <si>
-    <t>Freezer</t>
-  </si>
-  <si>
-    <t>Refrigerator/Freezer</t>
-  </si>
-  <si>
-    <t>temperature_monitoring_device</t>
-  </si>
-  <si>
-    <t>Temperature Monitoring Device</t>
-  </si>
-  <si>
-    <t>Is there a temperature monitoring device?</t>
-  </si>
-  <si>
-    <t>Dispositivo de monitoreo de temperatura</t>
-  </si>
-  <si>
-    <t>data('temperature_monitoring_device') === 'yes'</t>
-  </si>
-  <si>
-    <t>temperature_monitoring_device_functional_status</t>
-  </si>
-  <si>
-    <t>Temperature Monitoring Device Functional</t>
-  </si>
-  <si>
-    <t>Dispositivo de monitoreo de temperatura funcional</t>
-  </si>
-  <si>
-    <t>¿Funciona el dispositivo de monitoreo de temperatura?</t>
-  </si>
-  <si>
-    <t>¿Tiene el dispositivo de monitoreo de temperatura?</t>
-  </si>
-  <si>
-    <t>temperature_monitoring_device_type</t>
-  </si>
-  <si>
-    <t>Temperature Monitoring Device Type</t>
-  </si>
-  <si>
-    <t>Tipo de dispositivo de monitoreo de temperatura</t>
-  </si>
-  <si>
-    <t>What type of the temperature monitoring device is present?</t>
-  </si>
-  <si>
-    <t>¿Qué tipo de dispositivo de monitoreo de temperatura está presente?</t>
-  </si>
-  <si>
-    <t>Volúmen bruto</t>
-  </si>
-  <si>
-    <t>Ingrese el volumen bruto:</t>
-  </si>
-  <si>
-    <t>functioning</t>
-  </si>
-  <si>
-    <t>Functioning</t>
-  </si>
-  <si>
-    <t>Fonctionne</t>
-  </si>
-  <si>
-    <t>not_functioning</t>
-  </si>
-  <si>
-    <t>Not Functioning</t>
-  </si>
-  <si>
-    <t>No Functionando</t>
-  </si>
-  <si>
-    <t>Ne fonctionne pas</t>
-  </si>
-  <si>
-    <t>user_friendly_status</t>
-  </si>
-  <si>
-    <t>data('backup_generator') === 'yes'</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Notas</t>
-  </si>
-  <si>
-    <t>Enter notes</t>
-  </si>
-  <si>
-    <t>Introduce notas</t>
+    <t>Year must be between 1950 and the current year or 0 if unknown</t>
+  </si>
+  <si>
+    <t>El año debe ser entre 1950 y el año actual o 0 si se desconoce</t>
+  </si>
+  <si>
+    <t>Enter 0 if year is unknown</t>
+  </si>
+  <si>
+    <t>Ingrese 0 si el año es desconocido</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1535,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>0</v>
@@ -1543,19 +1543,19 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
     </row>
     <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1568,8 +1568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="J1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1615,7 +1615,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
@@ -1624,16 +1624,16 @@
         <v>9</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="P1" t="s">
         <v>11</v>
@@ -1657,7 +1657,7 @@
         <v>136</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1715,20 +1715,20 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="L6" s="16"/>
     </row>
@@ -1737,23 +1737,23 @@
         <v>24</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F7" t="s">
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="L7" s="17"/>
     </row>
@@ -1763,20 +1763,20 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="16" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="L8" s="16"/>
     </row>
@@ -1810,19 +1810,19 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H10" t="s">
+        <v>140</v>
+      </c>
+      <c r="J10" t="s">
+        <v>141</v>
+      </c>
+      <c r="K10" t="s">
         <v>142</v>
-      </c>
-      <c r="G10" t="s">
-        <v>143</v>
-      </c>
-      <c r="H10" t="s">
-        <v>144</v>
-      </c>
-      <c r="J10" t="s">
-        <v>145</v>
-      </c>
-      <c r="K10" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1846,19 +1846,19 @@
         <v>33</v>
       </c>
       <c r="M11" t="s">
-        <v>140</v>
+        <v>297</v>
       </c>
       <c r="N11" t="s">
-        <v>141</v>
+        <v>298</v>
       </c>
       <c r="T11" t="s">
         <v>135</v>
       </c>
       <c r="U11" t="s">
-        <v>138</v>
+        <v>295</v>
       </c>
       <c r="V11" t="s">
-        <v>137</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1881,25 +1881,25 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H14" t="s">
+        <v>184</v>
+      </c>
+      <c r="J14" t="s">
         <v>185</v>
       </c>
-      <c r="H14" t="s">
-        <v>188</v>
-      </c>
-      <c r="J14" t="s">
-        <v>189</v>
-      </c>
       <c r="K14" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="M14" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="N14" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1907,25 +1907,25 @@
         <v>130</v>
       </c>
       <c r="F15" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G15" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H15" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J15" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K15" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="M15" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="N15" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1933,25 +1933,25 @@
         <v>130</v>
       </c>
       <c r="F16" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G16" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H16" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="M16" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="N16" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1959,25 +1959,25 @@
         <v>26</v>
       </c>
       <c r="F17" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G17" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H17" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J17" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="K17" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="M17" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="N17" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2018,19 +2018,19 @@
         <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F21" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H21" t="s">
         <v>42</v>
       </c>
       <c r="J21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K21" t="s">
         <v>43</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="22" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" s="13" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E22" t="s">
         <v>44</v>
@@ -2097,22 +2097,22 @@
         <v>24</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
@@ -2120,7 +2120,7 @@
         <v>16</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
@@ -2128,19 +2128,19 @@
         <v>26</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="H28" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="K28" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
@@ -2151,19 +2151,19 @@
         <v>41</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="J29" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
@@ -2186,30 +2186,30 @@
         <v>24</v>
       </c>
       <c r="E33" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F33" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G33" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H33" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C34" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
@@ -2220,19 +2220,19 @@
         <v>41</v>
       </c>
       <c r="F35" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G35" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="H35" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J35" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="K35" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
@@ -2250,19 +2250,19 @@
         <v>26</v>
       </c>
       <c r="F38" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G38" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="H38" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="J38" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="K38" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2308,51 +2308,51 @@
         <v>7</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="E3" s="23"/>
     </row>
     <row r="4" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E4" s="23"/>
     </row>
@@ -2368,16 +2368,16 @@
         <v>41</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2385,16 +2385,16 @@
         <v>41</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2404,31 +2404,31 @@
     </row>
     <row r="9" spans="1:5" s="20" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E9" s="22"/>
     </row>
     <row r="10" spans="1:5" s="20" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E10" s="21"/>
     </row>
@@ -2451,13 +2451,13 @@
         <v>44</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2465,13 +2465,13 @@
         <v>44</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2479,13 +2479,13 @@
         <v>44</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2493,13 +2493,13 @@
         <v>44</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2507,13 +2507,13 @@
         <v>44</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2527,7 +2527,7 @@
         <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2535,13 +2535,13 @@
         <v>35</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E20" s="21"/>
     </row>
@@ -2550,13 +2550,13 @@
         <v>35</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E21" s="21"/>
     </row>
@@ -2565,13 +2565,13 @@
         <v>35</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E22" s="21"/>
     </row>
@@ -2580,13 +2580,13 @@
         <v>35</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E23" s="21"/>
     </row>
@@ -2595,20 +2595,20 @@
         <v>35</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E24" s="21"/>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
         <v>59</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="28" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
@@ -2636,7 +2636,7 @@
     </row>
     <row r="29" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B29" t="s">
         <v>51</v>
@@ -2783,16 +2783,16 @@
         <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
@@ -2878,7 +2878,7 @@
         <v>84</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2895,7 +2895,7 @@
         <v>84</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3015,7 +3015,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F1" t="s">
         <v>101</v>
@@ -3024,7 +3024,7 @@
         <v>102</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3032,7 +3032,7 @@
         <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3040,7 +3040,7 @@
         <v>104</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3056,10 +3056,10 @@
         <v>106</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3081,7 +3081,7 @@
         <v>110</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -3095,21 +3095,21 @@
         <v>113</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="G9" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="F9" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>257</v>
-      </c>
       <c r="H9" s="24" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3127,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3150,7 +3150,7 @@
         <v>134</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>212</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>